<commit_message>
fix formating on polyAisolation 05.25.20
</commit_message>
<xml_diff>
--- a/s1cDNASample/s1cDNASample_H.BROWN_05.25.20.xlsx
+++ b/s1cDNASample/s1cDNASample_H.BROWN_05.25.20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="16">
   <si>
     <t xml:space="preserve">rnaDate</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">05.25.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEBNextPoly(A)E7490L</t>
   </si>
   <si>
     <t xml:space="preserve">E7420L</t>
@@ -177,15 +174,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -243,13 +242,13 @@
         <v>13</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -275,13 +274,13 @@
         <v>13</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,13 +306,13 @@
         <v>13</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -339,13 +338,13 @@
         <v>13</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -371,13 +370,13 @@
         <v>13</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,13 +402,13 @@
         <v>13</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -435,13 +434,13 @@
         <v>13</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,13 +466,13 @@
         <v>13</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,13 +498,13 @@
         <v>13</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -531,13 +530,13 @@
         <v>13</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,13 +562,13 @@
         <v>13</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,13 +594,13 @@
         <v>13</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -627,13 +626,13 @@
         <v>13</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,13 +658,13 @@
         <v>13</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -691,13 +690,13 @@
         <v>13</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,13 +722,13 @@
         <v>13</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,13 +754,13 @@
         <v>13</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,13 +786,13 @@
         <v>13</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,13 +818,13 @@
         <v>13</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,13 +850,13 @@
         <v>13</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,13 +882,13 @@
         <v>13</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,13 +914,13 @@
         <v>13</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,13 +946,13 @@
         <v>13</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,13 +978,13 @@
         <v>13</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,13 +1010,13 @@
         <v>13</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,15 +1042,18 @@
         <v>13</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>